<commit_message>
2nd Commit: Update Processing Fee Rate
</commit_message>
<xml_diff>
--- a/AxiesBreedingCalculator/BreedingCalculatorInput.xlsx
+++ b/AxiesBreedingCalculator/BreedingCalculatorInput.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AxiesBreedingCalculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AxiesBreedingCalculator\AxiesBreedingCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD2A36E-0E3D-418A-8F2F-AE4BE5A38776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75228349-6027-4AA4-AE40-33A4EB4E7552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{FA90A740-C07E-4780-9847-C9CA7231456A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ETH Price</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Nimo</t>
-  </si>
-  <si>
-    <t>Kimhoo</t>
   </si>
   <si>
     <t>Name</t>
@@ -430,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DAA267-181E-4B1B-85D7-4A89808E1990}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +444,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -524,47 +521,6 @@
         <v>0.09</v>
       </c>
       <c r="M2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>1805</v>
-      </c>
-      <c r="C3">
-        <v>0.125</v>
-      </c>
-      <c r="D3">
-        <v>0.11</v>
-      </c>
-      <c r="E3">
-        <v>0.09</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.11</v>
-      </c>
-      <c r="H3">
-        <v>0.09</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.1</v>
-      </c>
-      <c r="K3">
-        <v>0.1</v>
-      </c>
-      <c r="L3">
-        <v>0.09</v>
-      </c>
-      <c r="M3">
         <v>2</v>
       </c>
     </row>

</xml_diff>